<commit_message>
Update upload template and firelds
</commit_message>
<xml_diff>
--- a/public/assets/download/participants_template.xlsx
+++ b/public/assets/download/participants_template.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/LGIHE/Dev/tms-laravel/public/assets/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3E8BD1-A466-4F49-B0C2-69D36F1ED2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792CE1AD-1697-2C42-9203-CAD12046BE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2960" windowWidth="27640" windowHeight="16940" xr2:uid="{2805116A-59DD-994D-88E8-7766838D4947}"/>
+    <workbookView xWindow="3160" yWindow="2400" windowWidth="27640" windowHeight="16940" xr2:uid="{2805116A-59DD-994D-88E8-7766838D4947}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>gender</t>
   </si>
@@ -61,20 +61,35 @@
     <t>phone</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>id_no</t>
+  </si>
+  <si>
+    <t>institution_ownership</t>
+  </si>
+  <si>
+    <t>subjects</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>education_level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADBAB0F-FE1F-D04C-AA11-ADFA3C6DE3D3}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,15 +444,17 @@
     <col min="4" max="4" width="8" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" customWidth="1"/>
-    <col min="9" max="9" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="7" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" customWidth="1"/>
+    <col min="12" max="12" width="15.5" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -455,19 +472,29 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add dates_attended to the participant upload template
</commit_message>
<xml_diff>
--- a/public/assets/download/participants_template.xlsx
+++ b/public/assets/download/participants_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/LGIHE/Dev/tms-laravel/public/assets/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792CE1AD-1697-2C42-9203-CAD12046BE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF1D5AF-79D9-4E45-8623-EA64D8B6A991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="2400" windowWidth="27640" windowHeight="16940" xr2:uid="{2805116A-59DD-994D-88E8-7766838D4947}"/>
+    <workbookView xWindow="-1120" yWindow="2620" windowWidth="29600" windowHeight="16940" xr2:uid="{2805116A-59DD-994D-88E8-7766838D4947}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>gender</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>education_level</t>
+  </si>
+  <si>
+    <t>dates_attended</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADBAB0F-FE1F-D04C-AA11-ADFA3C6DE3D3}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,9 +453,10 @@
     <col min="11" max="11" width="16.1640625" customWidth="1"/>
     <col min="12" max="12" width="15.5" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -491,6 +495,9 @@
       </c>
       <c r="M1" t="s">
         <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>